<commit_message>
Corregidos contadores y enlazado a Google Drive
</commit_message>
<xml_diff>
--- a/docs/data/data_XLS.xlsx
+++ b/docs/data/data_XLS.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccruz\Google Drive\06_GITHUB\LideresSociales\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB6330C-21BC-40D8-AB90-D5EA6E10500E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA137193-6EE1-4894-A521-1BCE1EC9C796}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lideres_DB_Geo_corr" sheetId="1" r:id="rId1"/>
+    <sheet name="data_lideres" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lideres_DB_Geo_corr!$A$1:$T$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_lideres!$A$1:$T$129</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="629">
   <si>
     <t>RAW</t>
   </si>
@@ -1966,14 +1967,23 @@
   <si>
     <t>&lt;p&gt; Alirio Antonio Arenas Gómez era un reconocido líder social en Ocaña por su trabajo en la zona rural de la vereda San Isidro, donde era presidente de la Junta de Acción Comunal. También hizo parte del Movimiento por la Constituyente Popular (MCP), y fue concejal y presidente del Concejo del municipio de Convención, por el partido MAIS. El pasado 2 de septiembre en la madrugada fue asesinado en el barrio Belén, de Ocaña, por hombres que le dispararon varias veces. Arenas había denunciado amenazas a su vida en los últimos meses, y aunque la Unidad Nacional de Protección (UNP) había autorizado un esquema de protección para él, no se lo asignaron. &lt;/p&gt;</t>
   </si>
+  <si>
+    <t>131. Norberto Jaramillo</t>
+  </si>
+  <si>
+    <t>Norberto Jaramillo</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tal como muchos de los casos que hemos denunciado en los últimos meses, hombres armados llegaron hasta la casa de este líder social y lo asesinaron con disparos de arma de fuego. Jaramillo era presidente de la Junta de Acción Comunal de la vereda La Envidia, zona rural del municipio antioqueño de Tarazá, y trabajaba en programas de sustitución de cultivos de uso ilícito en la zona. En esta área del norte de Antioquia hacen presencia grupos como Los Caparrapos y las AGC, que cobran extorsiones a quienes participan en sustitución de cultivos y realizan atentados.&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2487,14 +2497,14 @@
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -2852,13 +2862,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T131"/>
+  <dimension ref="A1:T132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G135" sqref="G135"/>
+      <selection pane="bottomRight" activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9673,7 +9683,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="12" t="str">
-        <f t="shared" ref="C98:C131" si="22">+TEXT(B98,"0000")</f>
+        <f t="shared" ref="C98:C132" si="22">+TEXT(B98,"0000")</f>
         <v>0097</v>
       </c>
       <c r="D98" s="4" t="s">
@@ -9686,7 +9696,7 @@
         <v>36</v>
       </c>
       <c r="G98" s="14" t="str">
-        <f t="shared" ref="G98:G131" si="23">+CONCATENATE(E98,", ",F98)</f>
+        <f t="shared" ref="G98:G132" si="23">+CONCATENATE(E98,", ",F98)</f>
         <v>Buenos Aires, Cauca</v>
       </c>
       <c r="H98" s="6">
@@ -9703,15 +9713,15 @@
         <v>02-07-2018</v>
       </c>
       <c r="L98" s="18">
-        <f t="shared" ref="L98:L130" si="24">+YEAR(J98)</f>
+        <f t="shared" ref="L98:L127" si="24">+YEAR(J98)</f>
         <v>2018</v>
       </c>
       <c r="M98" s="18">
-        <f t="shared" ref="M98:M129" si="25">+MONTH(J98)</f>
+        <f t="shared" ref="M98:M127" si="25">+MONTH(J98)</f>
         <v>7</v>
       </c>
       <c r="N98" s="18">
-        <f t="shared" ref="N98:N129" si="26">+DAY(J98)</f>
+        <f t="shared" ref="N98:N127" si="26">+DAY(J98)</f>
         <v>2</v>
       </c>
       <c r="O98" s="14" t="str">
@@ -11827,15 +11837,15 @@
         <v>25-08-2018</v>
       </c>
       <c r="L128" s="18">
-        <f t="shared" ref="L128:L131" si="29">+YEAR(J128)</f>
+        <f t="shared" ref="L128:L132" si="29">+YEAR(J128)</f>
         <v>2018</v>
       </c>
       <c r="M128" s="18">
-        <f t="shared" ref="M128:M131" si="30">+MONTH(J128)</f>
+        <f t="shared" ref="M128:M132" si="30">+MONTH(J128)</f>
         <v>8</v>
       </c>
       <c r="N128" s="18">
-        <f t="shared" ref="N128:N131" si="31">+DAY(J128)</f>
+        <f t="shared" ref="N128:N132" si="31">+DAY(J128)</f>
         <v>25</v>
       </c>
       <c r="O128" s="14" t="str">
@@ -11965,7 +11975,7 @@
         <v>43140</v>
       </c>
       <c r="K130" s="16" t="str">
-        <f t="shared" ref="K130:K131" si="32">+TEXT(J130,"DD-MM-YYYY")</f>
+        <f t="shared" ref="K130:K132" si="32">+TEXT(J130,"DD-MM-YYYY")</f>
         <v>09-02-2018</v>
       </c>
       <c r="L130" s="18">
@@ -12052,7 +12062,7 @@
         <v>31</v>
       </c>
       <c r="O131" s="14" t="str">
-        <f t="shared" ref="O131" si="34">+TEXT(K131,"DD-MMM-YYYY")</f>
+        <f t="shared" ref="O131:O132" si="34">+TEXT(K131,"DD-MMM-YYYY")</f>
         <v>31-08-2018</v>
       </c>
       <c r="P131" s="4" t="s">
@@ -12065,11 +12075,81 @@
         <v>19</v>
       </c>
       <c r="S131" s="14" t="str">
-        <f t="shared" ref="S131" si="35">+TEXT(CONCATENATE("data/IMG/",C131,".jpg"),)</f>
+        <f t="shared" ref="S131:S132" si="35">+TEXT(CONCATENATE("data/IMG/",C131,".jpg"),)</f>
         <v>data/IMG/0130.jpg</v>
       </c>
       <c r="T131" s="4" t="s">
         <v>624</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="B132" s="8">
+        <v>131</v>
+      </c>
+      <c r="C132" s="12" t="str">
+        <f t="shared" si="22"/>
+        <v>0131</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G132" s="14" t="str">
+        <f t="shared" si="23"/>
+        <v>Tarazá, Antioquia</v>
+      </c>
+      <c r="H132" s="6">
+        <v>-75.38</v>
+      </c>
+      <c r="I132" s="6">
+        <v>7.57</v>
+      </c>
+      <c r="J132" s="10">
+        <v>43348</v>
+      </c>
+      <c r="K132" s="16" t="str">
+        <f t="shared" si="32"/>
+        <v>05-09-2018</v>
+      </c>
+      <c r="L132" s="18">
+        <f t="shared" si="29"/>
+        <v>2018</v>
+      </c>
+      <c r="M132" s="18">
+        <f t="shared" si="30"/>
+        <v>9</v>
+      </c>
+      <c r="N132" s="18">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="O132" s="14" t="str">
+        <f t="shared" si="34"/>
+        <v>05-09-2018</v>
+      </c>
+      <c r="P132" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q132" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="R132" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S132" s="14" t="str">
+        <f t="shared" si="35"/>
+        <v>data/IMG/0131.jpg</v>
+      </c>
+      <c r="T132" s="4" t="s">
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>